<commit_message>
Started formatting changes to the BOM
</commit_message>
<xml_diff>
--- a/eagle/T06_LockBox_Bom-Exl_current.xlsx
+++ b/eagle/T06_LockBox_Bom-Exl_current.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="24460" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="T06_LockBox_Bom1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="194">
   <si>
     <t>Part</t>
   </si>
@@ -32,45 +37,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>PB2</t>
-  </si>
-  <si>
-    <t>PB3</t>
-  </si>
-  <si>
-    <t>PB4</t>
-  </si>
-  <si>
-    <t>PB5</t>
-  </si>
-  <si>
-    <t>PC4</t>
-  </si>
-  <si>
-    <t>PC5</t>
-  </si>
-  <si>
-    <t>PC6</t>
-  </si>
-  <si>
-    <t>PD2</t>
-  </si>
-  <si>
-    <t>PD4</t>
-  </si>
-  <si>
-    <t>PD5</t>
-  </si>
-  <si>
-    <t>SPICEMODEL</t>
-  </si>
-  <si>
-    <t>SPICEPREFIX</t>
-  </si>
-  <si>
-    <t>VOUT</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -83,12 +49,6 @@
     <t>C0805</t>
   </si>
   <si>
-    <t>CAPACITOR, European symbol</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -104,9 +64,6 @@
     <t>C4</t>
   </si>
   <si>
-    <t>CC1206</t>
-  </si>
-  <si>
     <t>C1206</t>
   </si>
   <si>
@@ -137,9 +94,6 @@
     <t>Sol_ctrl</t>
   </si>
   <si>
-    <t>PINHD-1X2</t>
-  </si>
-  <si>
     <t>1X02</t>
   </si>
   <si>
@@ -152,9 +106,6 @@
     <t>ICSP</t>
   </si>
   <si>
-    <t>PINHD-2X3</t>
-  </si>
-  <si>
     <t>2X03</t>
   </si>
   <si>
@@ -164,9 +115,6 @@
     <t>LCD</t>
   </si>
   <si>
-    <t>PINHD-2X4</t>
-  </si>
-  <si>
     <t>2X04</t>
   </si>
   <si>
@@ -176,9 +124,6 @@
     <t>UNUSED</t>
   </si>
   <si>
-    <t>PINHD-2X5</t>
-  </si>
-  <si>
     <t>2X05</t>
   </si>
   <si>
@@ -188,15 +133,9 @@
     <t>10k</t>
   </si>
   <si>
-    <t>R-US_R0805</t>
-  </si>
-  <si>
     <t>R0805</t>
   </si>
   <si>
-    <t>RESISTOR, American symbol</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -209,12 +148,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R-US_M0805</t>
-  </si>
-  <si>
-    <t>M0805</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
@@ -272,33 +205,6 @@
     <t>Atmel 8-bit Microcontroller</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/ATMEGA328-PU/ATMEGA328-PU-ND/2271026</t>
-  </si>
-  <si>
-    <t>GPIO</t>
-  </si>
-  <si>
-    <t>MOSI</t>
-  </si>
-  <si>
-    <t>MISO</t>
-  </si>
-  <si>
-    <t>SCK</t>
-  </si>
-  <si>
-    <t>SDA</t>
-  </si>
-  <si>
-    <t>SCL</t>
-  </si>
-  <si>
-    <t>RESET</t>
-  </si>
-  <si>
-    <t>INT0</t>
-  </si>
-  <si>
     <t>U$2</t>
   </si>
   <si>
@@ -314,9 +220,6 @@
     <t>497-3468-1-ND</t>
   </si>
   <si>
-    <t>3.3V</t>
-  </si>
-  <si>
     <t>U$3</t>
   </si>
   <si>
@@ -347,15 +250,9 @@
     <t>ETHERNET_JACK</t>
   </si>
   <si>
-    <t>MODJACK8</t>
-  </si>
-  <si>
     <t>8-Pin eithernet jack</t>
   </si>
   <si>
-    <t>Voltage</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -644,9 +541,6 @@
     <t>CL31B106KAHNNNE</t>
   </si>
   <si>
-    <t>Part Number</t>
-  </si>
-  <si>
     <t>1276-1804-1-ND</t>
   </si>
   <si>
@@ -684,16 +578,40 @@
   </si>
   <si>
     <t>P1.00KCCT-ND</t>
+  </si>
+  <si>
+    <t>PINHD</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>RESISTOR</t>
+  </si>
+  <si>
+    <t>RJ-45</t>
+  </si>
+  <si>
+    <t>Digikey Part Number</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>CAPACITOR - Ceramic</t>
+  </si>
+  <si>
+    <t>Voltage/Power Rating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -829,6 +747,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1127,7 +1061,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1170,18 +1104,46 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1210,11 +1172,31 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1514,971 +1496,864 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="2" max="2" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="37.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="3"/>
+    <col min="12" max="12" width="11.83203125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2"/>
-      <c r="I2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="J3" s="3">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.218</v>
+      </c>
+      <c r="L3" s="5">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O2" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R2" t="s">
+      <c r="E4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J4" s="3">
+        <v>10</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="S2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="T2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J5" s="3">
+        <v>10</v>
+      </c>
+      <c r="K5" s="3">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="U2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="V2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="J6" s="3">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.1336</v>
+      </c>
+      <c r="L6" s="5">
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J7" s="3">
+        <v>25</v>
+      </c>
+      <c r="K7" s="3">
+        <v>5.96E-2</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="X2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
-      <c r="A3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
-        <v>214</v>
-      </c>
-      <c r="H3" t="s">
-        <v>213</v>
-      </c>
-      <c r="I3">
+      <c r="B11" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="J15" s="3">
+        <v>50</v>
+      </c>
+      <c r="K15" s="3">
+        <v>4.82E-2</v>
+      </c>
+      <c r="L15" s="5">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J18" s="3">
         <v>10</v>
       </c>
-      <c r="J3">
-        <v>0.218</v>
-      </c>
-      <c r="K3" s="1">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="V3" t="s">
-        <v>23</v>
-      </c>
-      <c r="W3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>210</v>
-      </c>
-      <c r="H4" t="s">
-        <v>208</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1.98</v>
-      </c>
-      <c r="V4" t="s">
-        <v>23</v>
-      </c>
-      <c r="W4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="K18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="3">
+        <v>150</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="3">
+        <v>33</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="3">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H5" t="s">
-        <v>211</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0.71</v>
-      </c>
-      <c r="V5" t="s">
-        <v>23</v>
-      </c>
-      <c r="W5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>216</v>
-      </c>
-      <c r="H6" t="s">
-        <v>215</v>
-      </c>
-      <c r="I6">
-        <v>25</v>
-      </c>
-      <c r="J6">
-        <v>0.1336</v>
-      </c>
-      <c r="K6" s="1">
-        <v>3.34</v>
-      </c>
-      <c r="V6" t="s">
-        <v>23</v>
-      </c>
-      <c r="W6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>218</v>
-      </c>
-      <c r="H7" t="s">
-        <v>217</v>
-      </c>
-      <c r="I7">
-        <v>25</v>
-      </c>
-      <c r="J7">
-        <v>5.96E-2</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1.49</v>
-      </c>
-      <c r="V7" t="s">
-        <v>23</v>
-      </c>
-      <c r="W7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="V8" t="s">
-        <v>23</v>
-      </c>
-      <c r="W8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="V9" t="s">
-        <v>23</v>
-      </c>
-      <c r="W9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F21" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F22" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
-      <c r="A13" t="s">
+      <c r="D23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F23" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B24" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E13" t="s">
+      <c r="B25" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
-      <c r="A14" t="s">
+      <c r="B26" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
-      <c r="A15" t="s">
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E15" t="s">
+      <c r="B30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F15" t="s">
+      <c r="C30" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G15" t="s">
-        <v>220</v>
-      </c>
-      <c r="H15" t="s">
-        <v>219</v>
-      </c>
-      <c r="I15">
-        <v>50</v>
-      </c>
-      <c r="J15">
-        <v>4.82E-2</v>
-      </c>
-      <c r="K15" s="1">
-        <v>2.41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24">
-      <c r="A16" t="s">
+      <c r="D30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24">
-      <c r="A17" t="s">
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24">
-      <c r="A18" t="s">
+      <c r="B31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E18" t="s">
+      <c r="H31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" t="s">
-        <v>222</v>
-      </c>
-      <c r="H18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I18">
-        <v>10</v>
-      </c>
-      <c r="J18">
-        <v>0.1</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24">
-      <c r="A19" t="s">
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B19">
-        <v>150</v>
-      </c>
-      <c r="D19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
-      <c r="A20" t="s">
+      <c r="B32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B20">
-        <v>33</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24">
-      <c r="A21" t="s">
+      <c r="C32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B21">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24">
-      <c r="A22" t="s">
+      <c r="B33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24">
-      <c r="A23" t="s">
+      <c r="C33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" t="s">
-        <v>58</v>
-      </c>
-      <c r="F23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24">
-      <c r="A24" t="s">
+      <c r="G33" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24">
-      <c r="A25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24">
-      <c r="A26" t="s">
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24">
-      <c r="A27" t="s">
+      <c r="B34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C34" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E28" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24">
-      <c r="A29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24">
-      <c r="A30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" t="s">
-        <v>85</v>
-      </c>
-      <c r="J30" t="s">
-        <v>86</v>
-      </c>
-      <c r="K30" t="s">
-        <v>86</v>
-      </c>
-      <c r="L30" t="s">
-        <v>86</v>
-      </c>
-      <c r="M30" t="s">
-        <v>87</v>
-      </c>
-      <c r="N30" t="s">
-        <v>88</v>
-      </c>
-      <c r="O30" t="s">
-        <v>89</v>
-      </c>
-      <c r="P30" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>91</v>
-      </c>
-      <c r="R30" t="s">
-        <v>92</v>
-      </c>
-      <c r="S30" t="s">
-        <v>93</v>
-      </c>
-      <c r="T30" t="s">
-        <v>86</v>
-      </c>
-      <c r="U30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24">
-      <c r="A31" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" t="s">
-        <v>95</v>
-      </c>
-      <c r="E31" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" t="s">
-        <v>97</v>
-      </c>
-      <c r="H31" t="s">
-        <v>98</v>
-      </c>
-      <c r="X31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" t="s">
-        <v>104</v>
-      </c>
-      <c r="F33" t="s">
-        <v>105</v>
-      </c>
-      <c r="H33" t="s">
-        <v>106</v>
-      </c>
-      <c r="I33" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" t="s">
-        <v>109</v>
-      </c>
-      <c r="E34" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" t="s">
-        <v>111</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="I1:J1"/>
+  <mergeCells count="11">
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A139"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection sqref="A1:A139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="53.109375" customWidth="1"/>
+    <col min="1" max="1" width="53.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -2488,32 +2363,32 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:1">
@@ -2523,32 +2398,32 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1">
@@ -2558,32 +2433,32 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:1">
@@ -2593,27 +2468,27 @@
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -2623,32 +2498,32 @@
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -2658,27 +2533,27 @@
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -2693,27 +2568,27 @@
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>157</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:1">
@@ -2728,32 +2603,32 @@
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:1">
@@ -2768,27 +2643,27 @@
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:1">
@@ -2803,27 +2678,27 @@
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:1">
@@ -2838,32 +2713,32 @@
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:1">
@@ -2873,32 +2748,32 @@
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:1">
@@ -2908,32 +2783,32 @@
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
     </row>
     <row r="108" spans="1:1">
@@ -2943,32 +2818,32 @@
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:1">
@@ -2978,37 +2853,37 @@
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
     </row>
     <row r="123" spans="1:1">
@@ -3018,85 +2893,90 @@
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>